<commit_message>
added red coat, edit its entry in the Movie_list.xlsx
</commit_message>
<xml_diff>
--- a/Dataset/Movie_list.xlsx
+++ b/Dataset/Movie_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f0da054e76bb5fa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\PycharmProjects\video-object-detection\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{032134E6-AC0F-4262-A635-87CD76791EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F831C85-4C3A-4C1E-8F8D-450F397F069A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D9F55F-AB7D-49E1-81B0-61BC2BB61ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Title</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>007 Joe.png</t>
+  </si>
+  <si>
+    <t>Red Coat</t>
+  </si>
+  <si>
+    <t>https://movieleatherjackets.com/demi-lovato-i-love-me-song-red-coat/</t>
+  </si>
+  <si>
+    <t>demi_lovato_red_coat.png</t>
   </si>
 </sst>
 </file>
@@ -740,10 +749,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1046,7 +1051,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,16 +1209,16 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
+        <v>53</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1271,8 +1276,9 @@
     <hyperlink ref="D7" r:id="rId5" display="https://www.amazon.it/Giroscopio-Trottola-Giocattolo-Equilibrio-Prestazioni/dp/B07ZJ65BHR/ref=sr_1_fkmr0_2?keywords=amazing-trading+Argent%C3%A9+Vintage+Totem+bon+march%C3%A9+de+gros+plus+chaud+toupie+en+alliage+de+Zinc&amp;linkCode=ogi&amp;psc=1&amp;qid=1678297645&amp;sr=8-2-fkmr0&amp;th=1" xr:uid="{C5FCBEBC-1DB9-43EB-8A50-CC5226B95DF2}"/>
     <hyperlink ref="D9" r:id="rId6" xr:uid="{DB91A3E7-2B75-45DD-B52F-70FFB57A8FB5}"/>
     <hyperlink ref="D10" r:id="rId7" xr:uid="{C56E24D4-BDCC-43DD-924D-FE1F1105D48B}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{52FB50A7-D233-4128-8AE9-1929D96ABF45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated movie titles, uploaded files to db
</commit_message>
<xml_diff>
--- a/Dataset/Movie_list.xlsx
+++ b/Dataset/Movie_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\PycharmProjects\video-object-detection\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D9F55F-AB7D-49E1-81B0-61BC2BB61ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B2EC97-EC3B-4504-A038-89CF11B30018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,57 +40,30 @@
     <t>Product_images</t>
   </si>
   <si>
-    <t>Iron Man vs Loki - "We have a Hulk" - Suit Up Scene | The Avengers (2012) Movie Clip HD</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=NsRLOV4pHyk&amp;t=6s</t>
   </si>
   <si>
-    <t>Bruce Banner and Tony Stark put Jarvis Into Body - Avengers Age of Ultron (2015) Movie Clip HD Scene</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=kuvJRGrInPU</t>
   </si>
   <si>
-    <t>The Devil Wears Prada (4/5) Movie CLIP - Andy Gets a Makeover (2006) HD</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=HSPYgwP9R84</t>
   </si>
   <si>
-    <t>The Devil Wears Prada (2/5) Movie CLIP - Andy's Interview (2006) HD</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=b2f2Kqt_KcE</t>
   </si>
   <si>
-    <t>The Escape from Limbo, Inception ending, Deja Vu</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=a5R3_ToFRGg</t>
   </si>
   <si>
-    <t>Inception - Ending</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=XQPy88-E2zo</t>
   </si>
   <si>
-    <t>Demi Lovato - I Love Me (Official Video)</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=vImvzQCb0o8</t>
   </si>
   <si>
-    <t>Katy Perry - Hot N Cold (Official)</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=kTHNpusq654</t>
   </si>
   <si>
-    <t>NO TIME TO DIE (2021) | Nuovo Trailer ITA del film con 007</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=XCQaWwHIrkU</t>
   </si>
   <si>
@@ -121,9 +94,6 @@
     <t>DJ DRAGON CLASSIC HEATHER NAVY T-SHIRT</t>
   </si>
   <si>
-    <t>Louis Poulsen, blazer à détail de patch (2005)</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -166,9 +136,6 @@
     <t>DJ DRAGON CLASSIC HEATHER NAVY T-SHIRT.png</t>
   </si>
   <si>
-    <t>Louis Poulsen.png, blazer à détail de patch (2005).png</t>
-  </si>
-  <si>
     <t>Poltrona Willow di Charles Rennie Mackintosh.png</t>
   </si>
   <si>
@@ -188,6 +155,39 @@
   </si>
   <si>
     <t>demi_lovato_red_coat.png</t>
+  </si>
+  <si>
+    <t>iron man vs loki</t>
+  </si>
+  <si>
+    <t>avengers age of ultron</t>
+  </si>
+  <si>
+    <t>the devil wears prada andy's interview</t>
+  </si>
+  <si>
+    <t>the devil wears prada andy gets a makeover</t>
+  </si>
+  <si>
+    <t>inception ending</t>
+  </si>
+  <si>
+    <t>inception the escape from limbo</t>
+  </si>
+  <si>
+    <t>no time to die</t>
+  </si>
+  <si>
+    <t>hot n cold</t>
+  </si>
+  <si>
+    <t>i love me</t>
+  </si>
+  <si>
+    <t>Louis Poulsen.png, blazer with patch detail.png</t>
+  </si>
+  <si>
+    <t>Louis Poulsen, blazer with patch detail</t>
   </si>
 </sst>
 </file>
@@ -1051,14 +1051,16 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="64.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="118.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1083,182 +1085,182 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>